<commit_message>
ultima version revisada para ec2 aws
</commit_message>
<xml_diff>
--- a/src/public/uploads/Dependencias.xlsx
+++ b/src/public/uploads/Dependencias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliocesarmendoza/Desktop/pipApp/Backend-pi/src/public/uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcmendoza/Desktop/pipApp/sse-pdm/src/public/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE6F18A-BF51-FA48-BBC1-A5D5B193DB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47206B4-68F4-BD42-BC18-1F08EC3D236E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="5020" windowWidth="38400" windowHeight="19860" xr2:uid="{5D94F2EC-747A-1D48-9097-F1BC82C61895}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{5D94F2EC-747A-1D48-9097-F1BC82C61895}"/>
   </bookViews>
   <sheets>
     <sheet name="Dependencias" sheetId="1" r:id="rId1"/>
@@ -945,7 +945,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>